<commit_message>
CMMS file jobs annoniem gemaakt
</commit_message>
<xml_diff>
--- a/data/CMMS_demodata.xlsx
+++ b/data/CMMS_demodata.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Promotie\Papers\INEC2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70156138-5F82-4130-9B58-84682BEE26F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,9 +57,6 @@
     <t>SO</t>
   </si>
   <si>
-    <t>Bestellingen t.b.v. BUBO afsluiters</t>
-  </si>
-  <si>
     <t>40085158</t>
   </si>
   <si>
@@ -79,9 +75,6 @@
     <t>M1</t>
   </si>
   <si>
-    <t>1591 ZeKoWa P. BB + SB waaiers vervangen</t>
-  </si>
-  <si>
     <t>40506403</t>
   </si>
   <si>
@@ -148,16 +141,22 @@
     <t>x4</t>
   </si>
   <si>
-    <t>Voorbestelling LLI 3x Zekowa</t>
-  </si>
-  <si>
-    <t>BESTELORDER LLI 3X ZEKOWA</t>
+    <t>job description 1</t>
+  </si>
+  <si>
+    <t>job description 2</t>
+  </si>
+  <si>
+    <t>job description 3</t>
+  </si>
+  <si>
+    <t>job description 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
@@ -213,7 +212,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -490,76 +489,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -567,13 +566,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2">
         <v>42025</v>
@@ -595,27 +594,27 @@
         <v>42244</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N2" s="2">
         <v>42780</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2">
         <v>42474</v>
@@ -635,27 +634,27 @@
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N3" s="2">
         <v>42780</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F4" s="2">
         <v>42682</v>
@@ -679,27 +678,27 @@
         <v>42716</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N4" s="2">
         <v>42719</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2">
         <v>42705</v>
@@ -721,7 +720,7 @@
         <v>43084</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N5" s="2">
         <v>43285</v>

</xml_diff>